<commit_message>
Salmonella/Coccidia updation Signed-off-by: junaid.alam <junaid.alam@analytics.com.pk>
</commit_message>
<xml_diff>
--- a/Excel/MetaData RunMode1.xlsx
+++ b/Excel/MetaData RunMode1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="97">
   <si>
     <t>Result Date</t>
   </si>
@@ -158,12 +158,166 @@
   </si>
   <si>
     <t>TestAutomation3427</t>
+  </si>
+  <si>
+    <t>TestAutomation30227U</t>
+  </si>
+  <si>
+    <t>A0789107</t>
+  </si>
+  <si>
+    <t>TestCartridge0227</t>
+  </si>
+  <si>
+    <t>TestAutomation40227U</t>
+  </si>
+  <si>
+    <t>A0789112</t>
+  </si>
+  <si>
+    <t>TestAutomation20227U</t>
+  </si>
+  <si>
+    <t>A0789106</t>
+  </si>
+  <si>
+    <t>A0789111</t>
+  </si>
+  <si>
+    <t>TestAutomation10227U</t>
+  </si>
+  <si>
+    <t>A0789101</t>
+  </si>
+  <si>
+    <t>A0789108</t>
+  </si>
+  <si>
+    <t>A0789102</t>
+  </si>
+  <si>
+    <t>A0789103</t>
+  </si>
+  <si>
+    <t>A0789109</t>
+  </si>
+  <si>
+    <t>A0789104</t>
+  </si>
+  <si>
+    <t>A0789105</t>
+  </si>
+  <si>
+    <t>A0789110</t>
+  </si>
+  <si>
+    <t>TestAutomation14728U</t>
+  </si>
+  <si>
+    <t>A0789303</t>
+  </si>
+  <si>
+    <t>TestCartridge4728</t>
+  </si>
+  <si>
+    <t>A0789301</t>
+  </si>
+  <si>
+    <t>TestAutomation34728U</t>
+  </si>
+  <si>
+    <t>A0789307</t>
+  </si>
+  <si>
+    <t>TestAutomation44728U</t>
+  </si>
+  <si>
+    <t>A0789310</t>
+  </si>
+  <si>
+    <t>A0789308</t>
+  </si>
+  <si>
+    <t>A0789312</t>
+  </si>
+  <si>
+    <t>A0789302</t>
+  </si>
+  <si>
+    <t>TestAutomation24728U</t>
+  </si>
+  <si>
+    <t>A0789305</t>
+  </si>
+  <si>
+    <t>A0789309</t>
+  </si>
+  <si>
+    <t>A0789304</t>
+  </si>
+  <si>
+    <t>A0789311</t>
+  </si>
+  <si>
+    <t>A0789306</t>
+  </si>
+  <si>
+    <t>TestAutomation15813U</t>
+  </si>
+  <si>
+    <t>A0789802</t>
+  </si>
+  <si>
+    <t>TestCartridge5813</t>
+  </si>
+  <si>
+    <t>TestAutomation35813U</t>
+  </si>
+  <si>
+    <t>A0789808</t>
+  </si>
+  <si>
+    <t>TestAutomation45813U</t>
+  </si>
+  <si>
+    <t>A0789812</t>
+  </si>
+  <si>
+    <t>TestAutomation25813U</t>
+  </si>
+  <si>
+    <t>A0789805</t>
+  </si>
+  <si>
+    <t>A0789806</t>
+  </si>
+  <si>
+    <t>A0789810</t>
+  </si>
+  <si>
+    <t>A0789809</t>
+  </si>
+  <si>
+    <t>A0789803</t>
+  </si>
+  <si>
+    <t>A0789811</t>
+  </si>
+  <si>
+    <t>A0789804</t>
+  </si>
+  <si>
+    <t>A0789807</t>
+  </si>
+  <si>
+    <t>A0789801</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -549,16 +703,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.09765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="19.69921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="9.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.69921875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.09765625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.09765625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.69921875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.69921875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="9.5" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="10.69921875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -637,12 +791,14 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
       <c r="E2" t="s">
         <v>26</v>
       </c>
@@ -658,7 +814,9 @@
       <c r="L2" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="1"/>
+      <c r="R2" t="s">
+        <v>80</v>
+      </c>
       <c r="T2" t="s">
         <v>31</v>
       </c>
@@ -680,9 +838,11 @@
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
       <c r="E3" t="s">
         <v>26</v>
       </c>
@@ -698,7 +858,9 @@
       <c r="L3" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="1"/>
+      <c r="R3" t="s">
+        <v>83</v>
+      </c>
       <c r="T3" t="s">
         <v>31</v>
       </c>
@@ -717,12 +879,14 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
       <c r="E4" t="s">
         <v>26</v>
       </c>
@@ -738,7 +902,9 @@
       <c r="L4" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="1"/>
+      <c r="R4" t="s">
+        <v>85</v>
+      </c>
       <c r="T4" t="s">
         <v>31</v>
       </c>
@@ -757,12 +923,14 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D5" t="s">
+        <v>88</v>
+      </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
@@ -778,7 +946,9 @@
       <c r="L5" t="s">
         <v>29</v>
       </c>
-      <c r="R5" s="1"/>
+      <c r="R5" t="s">
+        <v>87</v>
+      </c>
       <c r="T5" t="s">
         <v>31</v>
       </c>
@@ -797,12 +967,14 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
       <c r="E6" t="s">
         <v>26</v>
       </c>
@@ -818,7 +990,9 @@
       <c r="L6" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="1"/>
+      <c r="R6" t="s">
+        <v>87</v>
+      </c>
       <c r="T6" t="s">
         <v>31</v>
       </c>
@@ -837,12 +1011,14 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D7" t="s">
+        <v>90</v>
+      </c>
       <c r="E7" t="s">
         <v>26</v>
       </c>
@@ -858,7 +1034,9 @@
       <c r="L7" t="s">
         <v>29</v>
       </c>
-      <c r="R7" s="1"/>
+      <c r="R7" t="s">
+        <v>85</v>
+      </c>
       <c r="T7" t="s">
         <v>31</v>
       </c>
@@ -877,12 +1055,14 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
       <c r="E8" t="s">
         <v>26</v>
       </c>
@@ -898,7 +1078,9 @@
       <c r="L8" t="s">
         <v>29</v>
       </c>
-      <c r="R8" s="1"/>
+      <c r="R8" t="s">
+        <v>83</v>
+      </c>
       <c r="T8" t="s">
         <v>31</v>
       </c>
@@ -917,12 +1099,14 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
       <c r="E9" t="s">
         <v>26</v>
       </c>
@@ -938,7 +1122,9 @@
       <c r="L9" t="s">
         <v>29</v>
       </c>
-      <c r="R9" s="1"/>
+      <c r="R9" t="s">
+        <v>80</v>
+      </c>
       <c r="T9" t="s">
         <v>31</v>
       </c>
@@ -957,12 +1143,14 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
+        <v>93</v>
+      </c>
       <c r="E10" t="s">
         <v>26</v>
       </c>
@@ -978,7 +1166,9 @@
       <c r="L10" t="s">
         <v>29</v>
       </c>
-      <c r="R10" s="1"/>
+      <c r="R10" t="s">
+        <v>85</v>
+      </c>
       <c r="T10" t="s">
         <v>31</v>
       </c>
@@ -997,12 +1187,14 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D11" t="s">
+        <v>94</v>
+      </c>
       <c r="E11" t="s">
         <v>26</v>
       </c>
@@ -1018,7 +1210,9 @@
       <c r="L11" t="s">
         <v>29</v>
       </c>
-      <c r="R11" s="1"/>
+      <c r="R11" t="s">
+        <v>87</v>
+      </c>
       <c r="T11" t="s">
         <v>31</v>
       </c>
@@ -1037,12 +1231,14 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D12" t="s">
+        <v>95</v>
+      </c>
       <c r="E12" t="s">
         <v>26</v>
       </c>
@@ -1058,7 +1254,9 @@
       <c r="L12" t="s">
         <v>29</v>
       </c>
-      <c r="R12" s="1"/>
+      <c r="R12" t="s">
+        <v>83</v>
+      </c>
       <c r="T12" t="s">
         <v>31</v>
       </c>
@@ -1077,12 +1275,14 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
       <c r="E13" t="s">
         <v>26</v>
       </c>
@@ -1098,7 +1298,9 @@
       <c r="L13" t="s">
         <v>29</v>
       </c>
-      <c r="R13" s="1"/>
+      <c r="R13" t="s">
+        <v>80</v>
+      </c>
       <c r="T13" t="s">
         <v>31</v>
       </c>

</xml_diff>